<commit_message>
ENH: Add Aug-25 RT notes from Thunderball
</commit_message>
<xml_diff>
--- a/MISO/Constraint Analyses/Top Congestion Reports/Aug-25_RT.xlsx
+++ b/MISO/Constraint Analyses/Top Congestion Reports/Aug-25_RT.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://roscommonanalytics-my.sharepoint.com/personal/lgraham_roscommonanalytics_com/Documents/Documents/Obsidian_Vault/MISO/Constraint Analyses/Top Congestion Reports/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\logan\Documents\logan-obsidian\MISO\Constraint Analyses\Top Congestion Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{FAF94919-6728-4B45-97BD-3617BDB9CF52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9AD9B142-3CF8-411B-BA1E-78AC033E0819}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5152D2C6-2D4D-4D5E-A714-8B00001A2A6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28695" yWindow="0" windowWidth="29010" windowHeight="31785" activeTab="1" xr2:uid="{9F15D29B-4962-4665-9A6F-04DAA09C42A3}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9F15D29B-4962-4665-9A6F-04DAA09C42A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Aug-25 RT Pk" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="105">
   <si>
     <t>cid</t>
   </si>
@@ -319,6 +319,39 @@
   </si>
   <si>
     <t>drivers</t>
+  </si>
+  <si>
+    <t>Wind transfer from MISO into SPP. OTP wind. Lisbon-Enderlin 69 kV outage.</t>
+  </si>
+  <si>
+    <t>Jamestown-Fargo-Sheyenne 230 kV outages. Center-Jamestown 345 kV outage. Eastward wind transfer.</t>
+  </si>
+  <si>
+    <t>Jamestown-Fargo-Sheyenne 230 kV outages. Center-Jamestown, Helena-Chub Lk-Hampton 345 kV outages. Eastward wind transfer.</t>
+  </si>
+  <si>
+    <t>Excess load in ALTW, MEC, NSP arising from weak wind generation. Excess generation in KCPL.</t>
+  </si>
+  <si>
+    <t>Center-Jamestown 345 kV outage. Monticello Outage. Emmons-Logan wind push.</t>
+  </si>
+  <si>
+    <t>Sheas Lk-Helena-Chub Lk-Hampton 345 kV outages. Mankato Energy Center push.</t>
+  </si>
+  <si>
+    <t>Weak Albany Solar, Grant County Solar, Quilt Block wind generation. Note the negative correlation between Grant County BESS and flows.</t>
+  </si>
+  <si>
+    <t>Severe (50%+) derate on 8/9/2025 in conjuction with the Center-Jamestown 345 kV and Roughrider-Mandan 230 kV outages.</t>
+  </si>
+  <si>
+    <t>Peach Garden-Rugby 230 kV, Center-Jamestown 345 kV outages. Rugby, Now Frontier, Velva wind push.</t>
+  </si>
+  <si>
+    <t>Sheas Lk-Helena-Chub Lk-Hampton 345 kV outages. Chub Lk TR 345/115 kV outage.</t>
+  </si>
+  <si>
+    <t>Kohlman-Coon Ck 345 kV, Apache-Apache Tap 115 kV outages. Sherco, Sherco Solar push. ROSE PL7, LXNGTON7, GOOSELK7, RAMSY 7 load.</t>
   </si>
 </sst>
 </file>
@@ -330,7 +363,7 @@
     <numFmt numFmtId="165" formatCode="#,##0.00_);[Red]\(#,##0.00\);_(* 0.00_)"/>
     <numFmt numFmtId="166" formatCode="[$-409]mmm\-yy;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -376,17 +409,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -723,28 +757,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7269D69B-4ABB-4E4D-8919-A634C2675602}">
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="O39" sqref="O39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="43.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="8.5" style="2" customWidth="1"/>
+    <col min="7" max="7" width="7.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="5" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="47.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="112.625" style="2" customWidth="1"/>
+    <col min="16" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -791,884 +826,914 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+    <row r="2" spans="1:15">
+      <c r="A2" s="3">
         <v>80559</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="3">
         <v>-1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="E2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="7">
-        <v>45870</v>
-      </c>
-      <c r="H2" s="4">
+      <c r="G2" s="8">
+        <v>45870</v>
+      </c>
+      <c r="H2" s="5">
         <v>175.33</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="5">
         <v>155</v>
       </c>
-      <c r="J2" s="4">
+      <c r="J2" s="5">
         <v>136.51</v>
       </c>
-      <c r="K2" s="4">
+      <c r="K2" s="5">
         <v>21158.38</v>
       </c>
-      <c r="L2" s="5">
+      <c r="L2" s="6">
         <v>62.97</v>
       </c>
-      <c r="M2" s="6">
+      <c r="M2" s="7">
         <v>0.46129999999999999</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="O2" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" s="3">
         <v>292300</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="3">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="E3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="7">
-        <v>45870</v>
-      </c>
-      <c r="H3" s="4">
+      <c r="G3" s="8">
+        <v>45870</v>
+      </c>
+      <c r="H3" s="5">
         <v>323.13</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="5">
         <v>42</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3" s="5">
         <v>472.66</v>
       </c>
-      <c r="K3" s="4">
+      <c r="K3" s="5">
         <v>19851.54</v>
       </c>
-      <c r="L3" s="5">
+      <c r="L3" s="6">
         <v>59.08</v>
       </c>
-      <c r="M3" s="6">
+      <c r="M3" s="7">
         <v>0.125</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N3" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="O3" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" s="3">
         <v>3816</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="3">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="E4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="7">
-        <v>45870</v>
-      </c>
-      <c r="H4" s="4">
+      <c r="G4" s="8">
+        <v>45870</v>
+      </c>
+      <c r="H4" s="5">
         <v>688.86</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="5">
         <v>28</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4" s="5">
         <v>671.71</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K4" s="5">
         <v>18807.830000000002</v>
       </c>
-      <c r="L4" s="5">
+      <c r="L4" s="6">
         <v>55.98</v>
       </c>
-      <c r="M4" s="6">
+      <c r="M4" s="7">
         <v>8.3299999999999999E-2</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N4" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="O4" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="3">
         <v>499463</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="3">
         <v>-1</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="E5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="7">
-        <v>45870</v>
-      </c>
-      <c r="H5" s="4">
+      <c r="G5" s="8">
+        <v>45870</v>
+      </c>
+      <c r="H5" s="5">
         <v>162.34</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="5">
         <v>135</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5" s="5">
         <v>129.44999999999999</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K5" s="5">
         <v>17475.59</v>
       </c>
-      <c r="L5" s="5">
+      <c r="L5" s="6">
         <v>52.01</v>
       </c>
-      <c r="M5" s="6">
+      <c r="M5" s="7">
         <v>0.40179999999999999</v>
       </c>
-      <c r="N5" t="s">
+      <c r="N5" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+    <row r="6" spans="1:15">
+      <c r="A6" s="3">
         <v>431124</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="3">
         <v>-1</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="E6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="7">
-        <v>45870</v>
-      </c>
-      <c r="H6" s="4">
+      <c r="G6" s="8">
+        <v>45870</v>
+      </c>
+      <c r="H6" s="5">
         <v>574.66</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="5">
         <v>23</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J6" s="5">
         <v>661.53</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K6" s="5">
         <v>15215.15</v>
       </c>
-      <c r="L6" s="5">
+      <c r="L6" s="6">
         <v>45.28</v>
       </c>
-      <c r="M6" s="6">
+      <c r="M6" s="7">
         <v>6.8400000000000002E-2</v>
       </c>
-      <c r="N6" t="s">
+      <c r="N6" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+      <c r="O6" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="3">
         <v>237044</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="3">
         <v>1</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="E7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="7">
-        <v>45870</v>
-      </c>
-      <c r="H7" s="4">
+      <c r="G7" s="8">
+        <v>45870</v>
+      </c>
+      <c r="H7" s="5">
         <v>357.3</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="5">
         <v>37</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J7" s="5">
         <v>392.57</v>
       </c>
-      <c r="K7" s="4">
+      <c r="K7" s="5">
         <v>14525</v>
       </c>
-      <c r="L7" s="5">
+      <c r="L7" s="6">
         <v>43.23</v>
       </c>
-      <c r="M7" s="6">
+      <c r="M7" s="7">
         <v>0.1101</v>
       </c>
-      <c r="N7" t="s">
+      <c r="N7" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+    <row r="8" spans="1:15">
+      <c r="A8" s="3">
         <v>496106</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="3">
         <v>1</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="E8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="7">
-        <v>45870</v>
-      </c>
-      <c r="H8" s="4">
+      <c r="G8" s="8">
+        <v>45870</v>
+      </c>
+      <c r="H8" s="5">
         <v>195.41</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="5">
         <v>157</v>
       </c>
-      <c r="J8" s="4">
+      <c r="J8" s="5">
         <v>91.98</v>
       </c>
-      <c r="K8" s="4">
+      <c r="K8" s="5">
         <v>14441.13</v>
       </c>
-      <c r="L8" s="5">
+      <c r="L8" s="6">
         <v>42.98</v>
       </c>
-      <c r="M8" s="6">
+      <c r="M8" s="7">
         <v>0.46729999999999999</v>
       </c>
-      <c r="N8" t="s">
+      <c r="N8" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+      <c r="O8" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="3">
         <v>353605</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="3">
         <v>1</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="E9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="7">
-        <v>45870</v>
-      </c>
-      <c r="H9" s="4">
+      <c r="G9" s="8">
+        <v>45870</v>
+      </c>
+      <c r="H9" s="5">
         <v>586.32000000000005</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="5">
         <v>14</v>
       </c>
-      <c r="J9" s="4">
+      <c r="J9" s="5">
         <v>1021.4</v>
       </c>
-      <c r="K9" s="4">
+      <c r="K9" s="5">
         <v>14299.6</v>
       </c>
-      <c r="L9" s="5">
+      <c r="L9" s="6">
         <v>42.56</v>
       </c>
-      <c r="M9" s="6">
+      <c r="M9" s="7">
         <v>4.1700000000000001E-2</v>
       </c>
-      <c r="N9" t="s">
+      <c r="N9" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+      <c r="O9" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="3">
         <v>28297</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="3">
         <v>-1</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="E10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="7">
-        <v>45870</v>
-      </c>
-      <c r="H10" s="4">
+      <c r="G10" s="8">
+        <v>45870</v>
+      </c>
+      <c r="H10" s="5">
         <v>319.51</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10" s="5">
         <v>33</v>
       </c>
-      <c r="J10" s="4">
+      <c r="J10" s="5">
         <v>350.4</v>
       </c>
-      <c r="K10" s="4">
+      <c r="K10" s="5">
         <v>11563.28</v>
       </c>
-      <c r="L10" s="5">
+      <c r="L10" s="6">
         <v>34.409999999999997</v>
       </c>
-      <c r="M10" s="6">
+      <c r="M10" s="7">
         <v>9.8199999999999996E-2</v>
       </c>
-      <c r="N10" t="s">
+      <c r="N10" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+      <c r="O10" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="3">
         <v>345080</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="3">
         <v>-1</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" t="s">
+      <c r="E11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G11" s="7">
-        <v>45870</v>
-      </c>
-      <c r="H11" s="4">
+      <c r="G11" s="8">
+        <v>45870</v>
+      </c>
+      <c r="H11" s="5">
         <v>458.6</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I11" s="5">
         <v>26</v>
       </c>
-      <c r="J11" s="4">
+      <c r="J11" s="5">
         <v>419.57</v>
       </c>
-      <c r="K11" s="4">
+      <c r="K11" s="5">
         <v>10908.85</v>
       </c>
-      <c r="L11" s="5">
+      <c r="L11" s="6">
         <v>32.47</v>
       </c>
-      <c r="M11" s="6">
+      <c r="M11" s="7">
         <v>7.7399999999999997E-2</v>
       </c>
-      <c r="N11" t="s">
+      <c r="N11" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+    <row r="12" spans="1:15">
+      <c r="A12" s="3">
         <v>215200</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="3">
         <v>1</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="E12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G12" s="7">
-        <v>45870</v>
-      </c>
-      <c r="H12" s="4">
+      <c r="G12" s="8">
+        <v>45870</v>
+      </c>
+      <c r="H12" s="5">
         <v>378.14</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12" s="5">
         <v>14</v>
       </c>
-      <c r="J12" s="4">
+      <c r="J12" s="5">
         <v>776.9</v>
       </c>
-      <c r="K12" s="4">
+      <c r="K12" s="5">
         <v>10876.56</v>
       </c>
-      <c r="L12" s="5">
+      <c r="L12" s="6">
         <v>32.369999999999997</v>
       </c>
-      <c r="M12" s="6">
+      <c r="M12" s="7">
         <v>4.1700000000000001E-2</v>
       </c>
-      <c r="N12" t="s">
+      <c r="N12" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
+      <c r="O12" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="3">
         <v>417169</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="3">
         <v>1</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="E13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="7">
-        <v>45870</v>
-      </c>
-      <c r="H13" s="4">
+      <c r="G13" s="8">
+        <v>45870</v>
+      </c>
+      <c r="H13" s="5">
         <v>458.42</v>
       </c>
-      <c r="I13" s="4">
+      <c r="I13" s="5">
         <v>9</v>
       </c>
-      <c r="J13" s="4">
+      <c r="J13" s="5">
         <v>1110.1400000000001</v>
       </c>
-      <c r="K13" s="4">
+      <c r="K13" s="5">
         <v>9991.26</v>
       </c>
-      <c r="L13" s="5">
+      <c r="L13" s="6">
         <v>29.74</v>
       </c>
-      <c r="M13" s="6">
+      <c r="M13" s="7">
         <v>2.6800000000000001E-2</v>
       </c>
-      <c r="N13" t="s">
+      <c r="N13" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+    <row r="14" spans="1:15">
+      <c r="A14" s="3">
         <v>80391</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="3">
         <v>1</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E14" t="s">
-        <v>16</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="E14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G14" s="7">
-        <v>45870</v>
-      </c>
-      <c r="H14" s="4">
+      <c r="G14" s="8">
+        <v>45870</v>
+      </c>
+      <c r="H14" s="5">
         <v>258.92</v>
       </c>
-      <c r="I14" s="4">
+      <c r="I14" s="5">
         <v>38</v>
       </c>
-      <c r="J14" s="4">
+      <c r="J14" s="5">
         <v>243.17</v>
       </c>
-      <c r="K14" s="4">
+      <c r="K14" s="5">
         <v>9240.35</v>
       </c>
-      <c r="L14" s="5">
+      <c r="L14" s="6">
         <v>27.5</v>
       </c>
-      <c r="M14" s="6">
+      <c r="M14" s="7">
         <v>0.11310000000000001</v>
       </c>
-      <c r="N14" t="s">
+      <c r="N14" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+    <row r="15" spans="1:15">
+      <c r="A15" s="3">
         <v>389806</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="3">
         <v>-1</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" t="s">
+      <c r="E15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G15" s="7">
-        <v>45870</v>
-      </c>
-      <c r="H15" s="4">
+      <c r="G15" s="8">
+        <v>45870</v>
+      </c>
+      <c r="H15" s="5">
         <v>663.52</v>
       </c>
-      <c r="I15" s="4">
+      <c r="I15" s="5">
         <v>8</v>
       </c>
-      <c r="J15" s="4">
+      <c r="J15" s="5">
         <v>1093.92</v>
       </c>
-      <c r="K15" s="4">
+      <c r="K15" s="5">
         <v>8751.36</v>
       </c>
-      <c r="L15" s="5">
+      <c r="L15" s="6">
         <v>26.05</v>
       </c>
-      <c r="M15" s="6">
+      <c r="M15" s="7">
         <v>2.3800000000000002E-2</v>
       </c>
-      <c r="N15" t="s">
+      <c r="N15" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
+    <row r="16" spans="1:15">
+      <c r="A16" s="3">
         <v>368274</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="3">
         <v>1</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E16" t="s">
-        <v>16</v>
-      </c>
-      <c r="F16" t="s">
+      <c r="E16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G16" s="7">
-        <v>45870</v>
-      </c>
-      <c r="H16" s="4">
+      <c r="G16" s="8">
+        <v>45870</v>
+      </c>
+      <c r="H16" s="5">
         <v>510.94</v>
       </c>
-      <c r="I16" s="4">
+      <c r="I16" s="5">
         <v>17</v>
       </c>
-      <c r="J16" s="4">
+      <c r="J16" s="5">
         <v>509.75</v>
       </c>
-      <c r="K16" s="4">
+      <c r="K16" s="5">
         <v>8665.69</v>
       </c>
-      <c r="L16" s="5">
+      <c r="L16" s="6">
         <v>25.79</v>
       </c>
-      <c r="M16" s="6">
+      <c r="M16" s="7">
         <v>5.0599999999999999E-2</v>
       </c>
-      <c r="N16" t="s">
+      <c r="N16" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
+      <c r="O16" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
+      <c r="A17" s="3">
         <v>256140</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="3">
         <v>0</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E17" t="s">
-        <v>16</v>
-      </c>
-      <c r="F17" t="s">
+      <c r="E17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G17" s="7">
-        <v>45870</v>
-      </c>
-      <c r="H17" s="4">
+      <c r="G17" s="8">
+        <v>45870</v>
+      </c>
+      <c r="H17" s="5">
         <v>632.03</v>
       </c>
-      <c r="I17" s="4">
+      <c r="I17" s="5">
         <v>22</v>
       </c>
-      <c r="J17" s="4">
+      <c r="J17" s="5">
         <v>385.92</v>
       </c>
-      <c r="K17" s="4">
+      <c r="K17" s="5">
         <v>8490.14</v>
       </c>
-      <c r="L17" s="5">
+      <c r="L17" s="6">
         <v>25.27</v>
       </c>
-      <c r="M17" s="6">
+      <c r="M17" s="7">
         <v>6.5500000000000003E-2</v>
       </c>
-      <c r="N17" t="s">
+      <c r="N17" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
+    <row r="18" spans="1:15">
+      <c r="A18" s="3">
         <v>227222</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="3">
         <v>-1</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F18" t="s">
+      <c r="E18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G18" s="7">
-        <v>45870</v>
-      </c>
-      <c r="H18" s="4">
+      <c r="G18" s="8">
+        <v>45870</v>
+      </c>
+      <c r="H18" s="5">
         <v>445</v>
       </c>
-      <c r="I18" s="4">
+      <c r="I18" s="5">
         <v>11</v>
       </c>
-      <c r="J18" s="4">
+      <c r="J18" s="5">
         <v>661.99</v>
       </c>
-      <c r="K18" s="4">
+      <c r="K18" s="5">
         <v>7281.87</v>
       </c>
-      <c r="L18" s="5">
+      <c r="L18" s="6">
         <v>21.67</v>
       </c>
-      <c r="M18" s="6">
+      <c r="M18" s="7">
         <v>3.27E-2</v>
       </c>
-      <c r="N18" t="s">
+      <c r="N18" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
+    <row r="19" spans="1:15">
+      <c r="A19" s="3">
         <v>454642</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="3">
         <v>-1</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E19" t="s">
-        <v>16</v>
-      </c>
-      <c r="F19" t="s">
+      <c r="E19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G19" s="7">
-        <v>45870</v>
-      </c>
-      <c r="H19" s="4">
+      <c r="G19" s="8">
+        <v>45870</v>
+      </c>
+      <c r="H19" s="5">
         <v>737.24</v>
       </c>
-      <c r="I19" s="4">
+      <c r="I19" s="5">
         <v>6</v>
       </c>
-      <c r="J19" s="4">
+      <c r="J19" s="5">
         <v>1194.44</v>
       </c>
-      <c r="K19" s="4">
+      <c r="K19" s="5">
         <v>7166.67</v>
       </c>
-      <c r="L19" s="5">
+      <c r="L19" s="6">
         <v>21.33</v>
       </c>
-      <c r="M19" s="6">
+      <c r="M19" s="7">
         <v>1.7899999999999999E-2</v>
       </c>
-      <c r="N19" t="s">
+      <c r="N19" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
+    <row r="20" spans="1:15">
+      <c r="A20" s="3">
         <v>288556</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="3">
         <v>1</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F20" t="s">
+      <c r="E20" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G20" s="7">
-        <v>45870</v>
-      </c>
-      <c r="H20" s="4">
+      <c r="G20" s="8">
+        <v>45870</v>
+      </c>
+      <c r="H20" s="5">
         <v>317.06</v>
       </c>
-      <c r="I20" s="4">
+      <c r="I20" s="5">
         <v>38</v>
       </c>
-      <c r="J20" s="4">
+      <c r="J20" s="5">
         <v>185.15</v>
       </c>
-      <c r="K20" s="4">
+      <c r="K20" s="5">
         <v>7035.6</v>
       </c>
-      <c r="L20" s="5">
+      <c r="L20" s="6">
         <v>20.94</v>
       </c>
-      <c r="M20" s="6">
+      <c r="M20" s="7">
         <v>0.11310000000000001</v>
       </c>
-      <c r="N20" t="s">
+      <c r="N20" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
+    <row r="21" spans="1:15">
+      <c r="A21" s="3">
         <v>314718</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="3">
         <v>1</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E21" t="s">
-        <v>16</v>
-      </c>
-      <c r="F21" t="s">
+      <c r="E21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G21" s="7">
-        <v>45870</v>
-      </c>
-      <c r="H21" s="4">
+      <c r="G21" s="8">
+        <v>45870</v>
+      </c>
+      <c r="H21" s="5">
         <v>128.33000000000001</v>
       </c>
-      <c r="I21" s="4">
+      <c r="I21" s="5">
         <v>38</v>
       </c>
-      <c r="J21" s="4">
+      <c r="J21" s="5">
         <v>181.04</v>
       </c>
-      <c r="K21" s="4">
+      <c r="K21" s="5">
         <v>6879.35</v>
       </c>
-      <c r="L21" s="5">
+      <c r="L21" s="6">
         <v>20.47</v>
       </c>
-      <c r="M21" s="6">
+      <c r="M21" s="7">
         <v>0.11310000000000001</v>
       </c>
-      <c r="N21" t="s">
+      <c r="N21" s="2" t="s">
         <v>71</v>
+      </c>
+      <c r="O21" s="2" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1680,27 +1745,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21AE0423-61E0-438F-A903-48961667CEB9}">
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="44.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="5" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="47.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="108.125" style="2" customWidth="1"/>
+    <col min="16" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="30">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1747,887 +1814,915 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+    <row r="2" spans="1:15">
+      <c r="A2" s="3">
         <v>368274</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="3">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="E2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G2" s="3">
-        <v>45870</v>
-      </c>
-      <c r="H2" s="4">
+      <c r="G2" s="4">
+        <v>45870</v>
+      </c>
+      <c r="H2" s="5">
         <v>546.65</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="5">
         <v>51</v>
       </c>
-      <c r="J2" s="4">
+      <c r="J2" s="5">
         <v>606.87</v>
       </c>
-      <c r="K2" s="4">
+      <c r="K2" s="5">
         <v>30950.28</v>
       </c>
-      <c r="L2" s="5">
+      <c r="L2" s="6">
         <v>75.86</v>
       </c>
-      <c r="M2" s="6">
+      <c r="M2" s="7">
         <v>0.125</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="O2" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" s="3">
         <v>499463</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="3">
         <v>-1</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="E3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G3" s="3">
-        <v>45870</v>
-      </c>
-      <c r="H3" s="4">
+      <c r="G3" s="4">
+        <v>45870</v>
+      </c>
+      <c r="H3" s="5">
         <v>279.89999999999998</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="5">
         <v>144</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3" s="5">
         <v>141.5</v>
       </c>
-      <c r="K3" s="4">
+      <c r="K3" s="5">
         <v>20375.560000000001</v>
       </c>
-      <c r="L3" s="5">
+      <c r="L3" s="6">
         <v>49.94</v>
       </c>
-      <c r="M3" s="6">
+      <c r="M3" s="7">
         <v>0.35289999999999999</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N3" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+    <row r="4" spans="1:15">
+      <c r="A4" s="3">
         <v>314718</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="3">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="E4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G4" s="3">
-        <v>45870</v>
-      </c>
-      <c r="H4" s="4">
+      <c r="G4" s="4">
+        <v>45870</v>
+      </c>
+      <c r="H4" s="5">
         <v>131.55000000000001</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="5">
         <v>42</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4" s="5">
         <v>209.95</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K4" s="5">
         <v>8818</v>
       </c>
-      <c r="L4" s="5">
+      <c r="L4" s="6">
         <v>21.61</v>
       </c>
-      <c r="M4" s="6">
+      <c r="M4" s="7">
         <v>0.10290000000000001</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N4" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="O4" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="3">
         <v>3816</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="3">
         <v>1</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="E5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G5" s="3">
-        <v>45870</v>
-      </c>
-      <c r="H5" s="4">
+      <c r="G5" s="4">
+        <v>45870</v>
+      </c>
+      <c r="H5" s="5">
         <v>473.46</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="5">
         <v>17</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5" s="5">
         <v>418.71</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K5" s="5">
         <v>7118.02</v>
       </c>
-      <c r="L5" s="5">
+      <c r="L5" s="6">
         <v>17.45</v>
       </c>
-      <c r="M5" s="6">
+      <c r="M5" s="7">
         <v>4.1700000000000001E-2</v>
       </c>
-      <c r="N5" t="s">
+      <c r="N5" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="O5" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="3">
         <v>496106</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="3">
         <v>1</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="E6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G6" s="3">
-        <v>45870</v>
-      </c>
-      <c r="H6" s="4">
+      <c r="G6" s="4">
+        <v>45870</v>
+      </c>
+      <c r="H6" s="5">
         <v>32.94</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="5">
         <v>193</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J6" s="5">
         <v>34.590000000000003</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K6" s="5">
         <v>6676.13</v>
       </c>
-      <c r="L6" s="5">
+      <c r="L6" s="6">
         <v>16.36</v>
       </c>
-      <c r="M6" s="6">
+      <c r="M6" s="7">
         <v>0.47299999999999998</v>
       </c>
-      <c r="N6" t="s">
+      <c r="N6" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+      <c r="O6" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="3">
         <v>80559</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="3">
         <v>-1</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="E7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G7" s="3">
-        <v>45870</v>
-      </c>
-      <c r="H7" s="4">
+      <c r="G7" s="4">
+        <v>45870</v>
+      </c>
+      <c r="H7" s="5">
         <v>157.97999999999999</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="5">
         <v>75</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J7" s="5">
         <v>81.47</v>
       </c>
-      <c r="K7" s="4">
+      <c r="K7" s="5">
         <v>6110.62</v>
       </c>
-      <c r="L7" s="5">
+      <c r="L7" s="6">
         <v>14.98</v>
       </c>
-      <c r="M7" s="6">
+      <c r="M7" s="7">
         <v>0.18390000000000001</v>
       </c>
-      <c r="N7" t="s">
+      <c r="N7" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+      <c r="O7" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="3">
         <v>28297</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="3">
         <v>-1</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="E8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G8" s="3">
-        <v>45870</v>
-      </c>
-      <c r="H8" s="4">
+      <c r="G8" s="4">
+        <v>45870</v>
+      </c>
+      <c r="H8" s="5">
         <v>209.88</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="5">
         <v>27</v>
       </c>
-      <c r="J8" s="4">
+      <c r="J8" s="5">
         <v>209</v>
       </c>
-      <c r="K8" s="4">
+      <c r="K8" s="5">
         <v>5642.96</v>
       </c>
-      <c r="L8" s="5">
+      <c r="L8" s="6">
         <v>13.83</v>
       </c>
-      <c r="M8" s="6">
+      <c r="M8" s="7">
         <v>6.6199999999999995E-2</v>
       </c>
-      <c r="N8" t="s">
+      <c r="N8" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+      <c r="O8" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="3">
         <v>292300</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="3">
         <v>1</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="E9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G9" s="3">
-        <v>45870</v>
-      </c>
-      <c r="H9" s="4">
+      <c r="G9" s="4">
+        <v>45870</v>
+      </c>
+      <c r="H9" s="5">
         <v>151.62</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="5">
         <v>22</v>
       </c>
-      <c r="J9" s="4">
+      <c r="J9" s="5">
         <v>154</v>
       </c>
-      <c r="K9" s="4">
+      <c r="K9" s="5">
         <v>3388.01</v>
       </c>
-      <c r="L9" s="5">
+      <c r="L9" s="6">
         <v>8.3000000000000007</v>
       </c>
-      <c r="M9" s="6">
+      <c r="M9" s="7">
         <v>5.3900000000000003E-2</v>
       </c>
-      <c r="N9" t="s">
+      <c r="N9" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+      <c r="O9" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="3">
         <v>249472</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="3">
         <v>1</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="E10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G10" s="3">
-        <v>45870</v>
-      </c>
-      <c r="H10" s="4">
+      <c r="G10" s="4">
+        <v>45870</v>
+      </c>
+      <c r="H10" s="5">
         <v>490.39</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10" s="5">
         <v>7</v>
       </c>
-      <c r="J10" s="4">
+      <c r="J10" s="5">
         <v>458.2</v>
       </c>
-      <c r="K10" s="4">
+      <c r="K10" s="5">
         <v>3207.41</v>
       </c>
-      <c r="L10" s="5">
+      <c r="L10" s="6">
         <v>7.86</v>
       </c>
-      <c r="M10" s="6">
+      <c r="M10" s="7">
         <v>1.72E-2</v>
       </c>
-      <c r="N10" t="s">
+      <c r="N10" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+    <row r="11" spans="1:15">
+      <c r="A11" s="3">
         <v>311974</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="3">
         <v>-1</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" t="s">
+      <c r="E11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G11" s="3">
-        <v>45870</v>
-      </c>
-      <c r="H11" s="4">
+      <c r="G11" s="4">
+        <v>45870</v>
+      </c>
+      <c r="H11" s="5">
         <v>174.81</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I11" s="5">
         <v>21</v>
       </c>
-      <c r="J11" s="4">
+      <c r="J11" s="5">
         <v>149.38</v>
       </c>
-      <c r="K11" s="4">
+      <c r="K11" s="5">
         <v>3136.92</v>
       </c>
-      <c r="L11" s="5">
+      <c r="L11" s="6">
         <v>7.69</v>
       </c>
-      <c r="M11" s="6">
+      <c r="M11" s="7">
         <v>5.1499999999999997E-2</v>
       </c>
-      <c r="N11" t="s">
+      <c r="N11" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+    <row r="12" spans="1:15">
+      <c r="A12" s="3">
         <v>431124</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="3">
         <v>-1</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="E12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G12" s="3">
-        <v>45870</v>
-      </c>
-      <c r="H12" s="4">
+      <c r="G12" s="4">
+        <v>45870</v>
+      </c>
+      <c r="H12" s="5">
         <v>302.47000000000003</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12" s="5">
         <v>9</v>
       </c>
-      <c r="J12" s="4">
+      <c r="J12" s="5">
         <v>347.84</v>
       </c>
-      <c r="K12" s="4">
+      <c r="K12" s="5">
         <v>3130.55</v>
       </c>
-      <c r="L12" s="5">
+      <c r="L12" s="6">
         <v>7.67</v>
       </c>
-      <c r="M12" s="6">
+      <c r="M12" s="7">
         <v>2.2100000000000002E-2</v>
       </c>
-      <c r="N12" t="s">
+      <c r="N12" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
+      <c r="O12" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="3">
         <v>80391</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="3">
         <v>1</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="E13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G13" s="3">
-        <v>45870</v>
-      </c>
-      <c r="H13" s="4">
+      <c r="G13" s="4">
+        <v>45870</v>
+      </c>
+      <c r="H13" s="5">
         <v>282.38</v>
       </c>
-      <c r="I13" s="4">
+      <c r="I13" s="5">
         <v>15</v>
       </c>
-      <c r="J13" s="4">
+      <c r="J13" s="5">
         <v>194.98</v>
       </c>
-      <c r="K13" s="4">
+      <c r="K13" s="5">
         <v>2924.73</v>
       </c>
-      <c r="L13" s="5">
+      <c r="L13" s="6">
         <v>7.17</v>
       </c>
-      <c r="M13" s="6">
+      <c r="M13" s="7">
         <v>3.6799999999999999E-2</v>
       </c>
-      <c r="N13" t="s">
+      <c r="N13" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+    <row r="14" spans="1:15">
+      <c r="A14" s="3">
         <v>334192</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="3">
         <v>1</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E14" t="s">
-        <v>16</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="E14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G14" s="3">
-        <v>45870</v>
-      </c>
-      <c r="H14" s="4">
+      <c r="G14" s="4">
+        <v>45870</v>
+      </c>
+      <c r="H14" s="5">
         <v>137.37</v>
       </c>
-      <c r="I14" s="4">
+      <c r="I14" s="5">
         <v>18</v>
       </c>
-      <c r="J14" s="4">
+      <c r="J14" s="5">
         <v>159.80000000000001</v>
       </c>
-      <c r="K14" s="4">
+      <c r="K14" s="5">
         <v>2876.33</v>
       </c>
-      <c r="L14" s="5">
+      <c r="L14" s="6">
         <v>7.05</v>
       </c>
-      <c r="M14" s="6">
+      <c r="M14" s="7">
         <v>4.41E-2</v>
       </c>
-      <c r="N14" t="s">
+      <c r="N14" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+    <row r="15" spans="1:15">
+      <c r="A15" s="3">
         <v>334068</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="3">
         <v>1</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" t="s">
+      <c r="E15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G15" s="3">
-        <v>45870</v>
-      </c>
-      <c r="H15" s="4">
+      <c r="G15" s="4">
+        <v>45870</v>
+      </c>
+      <c r="H15" s="5">
         <v>80.34</v>
       </c>
-      <c r="I15" s="4">
+      <c r="I15" s="5">
         <v>30</v>
       </c>
-      <c r="J15" s="4">
+      <c r="J15" s="5">
         <v>92.94</v>
       </c>
-      <c r="K15" s="4">
+      <c r="K15" s="5">
         <v>2788.15</v>
       </c>
-      <c r="L15" s="5">
+      <c r="L15" s="6">
         <v>6.83</v>
       </c>
-      <c r="M15" s="6">
+      <c r="M15" s="7">
         <v>7.3499999999999996E-2</v>
       </c>
-      <c r="N15" t="s">
+      <c r="N15" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
+    <row r="16" spans="1:15">
+      <c r="A16" s="3">
         <v>215200</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="3">
         <v>1</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E16" t="s">
-        <v>16</v>
-      </c>
-      <c r="F16" t="s">
+      <c r="E16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G16" s="3">
-        <v>45870</v>
-      </c>
-      <c r="H16" s="4">
+      <c r="G16" s="4">
+        <v>45870</v>
+      </c>
+      <c r="H16" s="5">
         <v>617.14</v>
       </c>
-      <c r="I16" s="4">
+      <c r="I16" s="5">
         <v>4</v>
       </c>
-      <c r="J16" s="4">
+      <c r="J16" s="5">
         <v>642.66999999999996</v>
       </c>
-      <c r="K16" s="4">
+      <c r="K16" s="5">
         <v>2570.6799999999998</v>
       </c>
-      <c r="L16" s="5">
+      <c r="L16" s="6">
         <v>6.3</v>
       </c>
-      <c r="M16" s="6">
+      <c r="M16" s="7">
         <v>9.7999999999999997E-3</v>
       </c>
-      <c r="N16" t="s">
+      <c r="N16" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
+      <c r="O16" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" s="3">
         <v>345080</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="3">
         <v>-1</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E17" t="s">
-        <v>16</v>
-      </c>
-      <c r="F17" t="s">
+      <c r="E17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G17" s="3">
-        <v>45870</v>
-      </c>
-      <c r="H17" s="4">
+      <c r="G17" s="4">
+        <v>45870</v>
+      </c>
+      <c r="H17" s="5">
         <v>575.16999999999996</v>
       </c>
-      <c r="I17" s="4">
+      <c r="I17" s="5">
         <v>4</v>
       </c>
-      <c r="J17" s="4">
+      <c r="J17" s="5">
         <v>630.51</v>
       </c>
-      <c r="K17" s="4">
+      <c r="K17" s="5">
         <v>2522.0500000000002</v>
       </c>
-      <c r="L17" s="5">
+      <c r="L17" s="6">
         <v>6.18</v>
       </c>
-      <c r="M17" s="6">
+      <c r="M17" s="7">
         <v>9.7999999999999997E-3</v>
       </c>
-      <c r="N17" t="s">
+      <c r="N17" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
+    <row r="18" spans="1:14">
+      <c r="A18" s="3">
         <v>237044</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="3">
         <v>1</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F18" t="s">
+      <c r="E18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G18" s="3">
-        <v>45870</v>
-      </c>
-      <c r="H18" s="4">
+      <c r="G18" s="4">
+        <v>45870</v>
+      </c>
+      <c r="H18" s="5">
         <v>381.43</v>
       </c>
-      <c r="I18" s="4">
+      <c r="I18" s="5">
         <v>8</v>
       </c>
-      <c r="J18" s="4">
+      <c r="J18" s="5">
         <v>305.85000000000002</v>
       </c>
-      <c r="K18" s="4">
+      <c r="K18" s="5">
         <v>2446.8200000000002</v>
       </c>
-      <c r="L18" s="5">
+      <c r="L18" s="6">
         <v>6</v>
       </c>
-      <c r="M18" s="6">
+      <c r="M18" s="7">
         <v>1.9599999999999999E-2</v>
       </c>
-      <c r="N18" t="s">
+      <c r="N18" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
+    <row r="19" spans="1:14">
+      <c r="A19" s="3">
         <v>415037</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="3">
         <v>-1</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E19" t="s">
-        <v>16</v>
-      </c>
-      <c r="F19" t="s">
+      <c r="E19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G19" s="3">
-        <v>45870</v>
-      </c>
-      <c r="H19" s="4">
+      <c r="G19" s="4">
+        <v>45870</v>
+      </c>
+      <c r="H19" s="5">
         <v>272.83999999999997</v>
       </c>
-      <c r="I19" s="4">
+      <c r="I19" s="5">
         <v>6</v>
       </c>
-      <c r="J19" s="4">
+      <c r="J19" s="5">
         <v>398.85</v>
       </c>
-      <c r="K19" s="4">
+      <c r="K19" s="5">
         <v>2393.09</v>
       </c>
-      <c r="L19" s="5">
+      <c r="L19" s="6">
         <v>5.87</v>
       </c>
-      <c r="M19" s="6">
+      <c r="M19" s="7">
         <v>1.47E-2</v>
       </c>
-      <c r="N19" t="s">
+      <c r="N19" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
+    <row r="20" spans="1:14">
+      <c r="A20" s="3">
         <v>232780</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="3">
         <v>1</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="E20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F20" t="s">
+      <c r="E20" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G20" s="3">
-        <v>45870</v>
-      </c>
-      <c r="H20" s="4">
+      <c r="G20" s="4">
+        <v>45870</v>
+      </c>
+      <c r="H20" s="5">
         <v>88.77</v>
       </c>
-      <c r="I20" s="4">
+      <c r="I20" s="5">
         <v>30</v>
       </c>
-      <c r="J20" s="4">
+      <c r="J20" s="5">
         <v>75.41</v>
       </c>
-      <c r="K20" s="4">
+      <c r="K20" s="5">
         <v>2262.39</v>
       </c>
-      <c r="L20" s="5">
+      <c r="L20" s="6">
         <v>5.55</v>
       </c>
-      <c r="M20" s="6">
+      <c r="M20" s="7">
         <v>7.3599999999999999E-2</v>
       </c>
-      <c r="N20" t="s">
+      <c r="N20" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
+    <row r="21" spans="1:14">
+      <c r="A21" s="3">
         <v>197146</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="3">
         <v>1</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E21" t="s">
-        <v>16</v>
-      </c>
-      <c r="F21" t="s">
+      <c r="E21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G21" s="3">
-        <v>45870</v>
-      </c>
-      <c r="H21" s="4">
+      <c r="G21" s="4">
+        <v>45870</v>
+      </c>
+      <c r="H21" s="5">
         <v>175.64</v>
       </c>
-      <c r="I21" s="4">
+      <c r="I21" s="5">
         <v>14</v>
       </c>
-      <c r="J21" s="4">
+      <c r="J21" s="5">
         <v>154.24</v>
       </c>
-      <c r="K21" s="4">
+      <c r="K21" s="5">
         <v>2159.37</v>
       </c>
-      <c r="L21" s="5">
+      <c r="L21" s="6">
         <v>5.29</v>
       </c>
-      <c r="M21" s="6">
+      <c r="M21" s="7">
         <v>3.4299999999999997E-2</v>
       </c>
-      <c r="N21" t="s">
+      <c r="N21" s="2" t="s">
         <v>92</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>